<commit_message>
removed specific notebooks, added general case notebook
</commit_message>
<xml_diff>
--- a/DS1/GM/GM_10cov_sim.xlsx
+++ b/DS1/GM/GM_10cov_sim.xlsx
@@ -78,25 +78,25 @@
         <v>1.0</v>
       </c>
       <c r="F1" t="n">
-        <v>0.06866756406041494</v>
+        <v>0.05750029602107444</v>
       </c>
       <c r="G1" t="n">
-        <v>1.5078360763406158</v>
+        <v>0.07020772298987588</v>
       </c>
       <c r="H1" t="n">
-        <v>0.5505769369526616</v>
+        <v>0.625818588736696</v>
       </c>
       <c r="I1" t="n">
-        <v>0.05462919457625944</v>
+        <v>0.05756203460963144</v>
       </c>
       <c r="J1" t="n">
-        <v>0.3815824403852943</v>
+        <v>1.6247340862779955</v>
       </c>
       <c r="K1" t="n">
-        <v>0.8537844541420134</v>
+        <v>0.17303792644239602</v>
       </c>
       <c r="L1" t="n">
-        <v>0.42108027473252996</v>
+        <v>3.6881204119295345</v>
       </c>
     </row>
     <row r="2">
@@ -104,7 +104,7 @@
         <v>2.0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0619</v>
@@ -116,25 +116,25 @@
         <v>0.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.08004749934726337</v>
+        <v>0.06702953528633723</v>
       </c>
       <c r="G2" t="n">
-        <v>7.539180381703079</v>
+        <v>0.3510386149493794</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.063682620419406</v>
+        <v>0.06710150550538956</v>
       </c>
       <c r="J2" t="n">
-        <v>1.9079122019264716</v>
+        <v>8.123670431389979</v>
       </c>
       <c r="K2" t="n">
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>2.10540137366265</v>
+        <v>18.440602059647674</v>
       </c>
     </row>
     <row r="3">
@@ -154,25 +154,25 @@
         <v>0.5</v>
       </c>
       <c r="F3" t="n">
-        <v>0.20432156537750584</v>
+        <v>0.17109315953540039</v>
       </c>
       <c r="G3" t="n">
-        <v>0.37695901908515395</v>
+        <v>0.01755193074746897</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2752884684763308</v>
+        <v>0.312909294368348</v>
       </c>
       <c r="I3" t="n">
-        <v>0.16255014582013166</v>
+        <v>0.17127686381020277</v>
       </c>
       <c r="J3" t="n">
-        <v>0.09539561009632358</v>
+        <v>0.4061835215694989</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4268922270710067</v>
+        <v>0.08651896322119801</v>
       </c>
       <c r="L3" t="n">
-        <v>0.10527006868313249</v>
+        <v>0.9220301029823836</v>
       </c>
     </row>
     <row r="4">
@@ -192,25 +192,25 @@
         <v>0.5</v>
       </c>
       <c r="F4" t="n">
-        <v>0.10474713161758212</v>
+        <v>0.08771231596435083</v>
       </c>
       <c r="G4" t="n">
-        <v>0.37695901908515395</v>
+        <v>0.01755193074746897</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2752884684763308</v>
+        <v>0.312909294368348</v>
       </c>
       <c r="I4" t="n">
-        <v>0.08333266969259914</v>
+        <v>0.08780649347231914</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09539561009632358</v>
+        <v>0.4061835215694989</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4268922270710067</v>
+        <v>0.08651896322119801</v>
       </c>
       <c r="L4" t="n">
-        <v>0.10527006868313249</v>
+        <v>0.9220301029823836</v>
       </c>
     </row>
     <row r="5">
@@ -218,7 +218,7 @@
         <v>5.0</v>
       </c>
       <c r="B5" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C5" t="n">
         <v>1.046</v>
@@ -230,25 +230,25 @@
         <v>2.0</v>
       </c>
       <c r="F5" t="n">
-        <v>1.3526604897776653</v>
+        <v>1.1326800308482836</v>
       </c>
       <c r="G5" t="n">
-        <v>12.062688610724926</v>
+        <v>0.561661783919007</v>
       </c>
       <c r="H5" t="n">
-        <v>1.1011538739053233</v>
+        <v>1.251637177473392</v>
       </c>
       <c r="I5" t="n">
-        <v>1.0761231172649224</v>
+        <v>1.1338961996548866</v>
       </c>
       <c r="J5" t="n">
-        <v>3.0526595230823546</v>
+        <v>12.997872690223964</v>
       </c>
       <c r="K5" t="n">
-        <v>1.7075689082840269</v>
+        <v>0.34607585288479203</v>
       </c>
       <c r="L5" t="n">
-        <v>3.3686421978602397</v>
+        <v>29.504963295436276</v>
       </c>
     </row>
     <row r="6">
@@ -256,7 +256,7 @@
         <v>6.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C6" t="n">
         <v>1.75</v>
@@ -268,25 +268,25 @@
         <v>5.0</v>
       </c>
       <c r="F6" t="n">
-        <v>2.2630553127255393</v>
+        <v>1.8950191720693081</v>
       </c>
       <c r="G6" t="n">
-        <v>12.062688610724926</v>
+        <v>0.561661783919007</v>
       </c>
       <c r="H6" t="n">
-        <v>2.752884684763308</v>
+        <v>3.1290929436834802</v>
       </c>
       <c r="I6" t="n">
-        <v>1.800397184716648</v>
+        <v>1.897053871315537</v>
       </c>
       <c r="J6" t="n">
-        <v>3.0526595230823546</v>
+        <v>12.997872690223964</v>
       </c>
       <c r="K6" t="n">
-        <v>4.268922270710068</v>
+        <v>0.8651896322119801</v>
       </c>
       <c r="L6" t="n">
-        <v>3.3686421978602397</v>
+        <v>29.504963295436276</v>
       </c>
     </row>
     <row r="7">
@@ -294,7 +294,7 @@
         <v>7.0</v>
       </c>
       <c r="B7" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C7" t="n">
         <v>2.96</v>
@@ -306,25 +306,25 @@
         <v>4.5</v>
       </c>
       <c r="F7" t="n">
-        <v>3.827796414667198</v>
+        <v>3.205289571042944</v>
       </c>
       <c r="G7" t="n">
-        <v>9.047016458043695</v>
+        <v>0.42124633793925526</v>
       </c>
       <c r="H7" t="n">
-        <v>2.4775962162869773</v>
+        <v>2.816183649315132</v>
       </c>
       <c r="I7" t="n">
-        <v>3.0452432381493018</v>
+        <v>3.20873111948228</v>
       </c>
       <c r="J7" t="n">
-        <v>2.289494642311766</v>
+        <v>9.748404517667973</v>
       </c>
       <c r="K7" t="n">
-        <v>3.8420300436390606</v>
+        <v>0.7786706689907821</v>
       </c>
       <c r="L7" t="n">
-        <v>2.5264816483951797</v>
+        <v>22.128722471577206</v>
       </c>
     </row>
     <row r="8">
@@ -332,7 +332,7 @@
         <v>8.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C8" t="n">
         <v>4.97</v>
@@ -344,25 +344,25 @@
         <v>2.5</v>
       </c>
       <c r="F8" t="n">
-        <v>6.427077088140532</v>
+        <v>5.381854448676835</v>
       </c>
       <c r="G8" t="n">
-        <v>9.047016458043695</v>
+        <v>0.42124633793925526</v>
       </c>
       <c r="H8" t="n">
-        <v>1.376442342381654</v>
+        <v>1.5645464718417401</v>
       </c>
       <c r="I8" t="n">
-        <v>5.11312800459528</v>
+        <v>5.3876329945361245</v>
       </c>
       <c r="J8" t="n">
-        <v>2.289494642311766</v>
+        <v>9.748404517667973</v>
       </c>
       <c r="K8" t="n">
-        <v>2.134461135355034</v>
+        <v>0.43259481610599004</v>
       </c>
       <c r="L8" t="n">
-        <v>2.5264816483951797</v>
+        <v>22.128722471577206</v>
       </c>
     </row>
     <row r="9">
@@ -382,25 +382,25 @@
         <v>4.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5431332750541294</v>
+        <v>0.4548046012966339</v>
       </c>
       <c r="G9" t="n">
-        <v>9.047016458043695</v>
+        <v>0.42124633793925526</v>
       </c>
       <c r="H9" t="n">
-        <v>2.2023077478106465</v>
+        <v>2.503274354946784</v>
       </c>
       <c r="I9" t="n">
-        <v>0.43209532433199555</v>
+        <v>0.4552929291157289</v>
       </c>
       <c r="J9" t="n">
-        <v>2.289494642311766</v>
+        <v>9.748404517667973</v>
       </c>
       <c r="K9" t="n">
-        <v>3.4151378165680537</v>
+        <v>0.6921517057695841</v>
       </c>
       <c r="L9" t="n">
-        <v>2.5264816483951797</v>
+        <v>22.128722471577206</v>
       </c>
     </row>
     <row r="10">
@@ -420,25 +420,25 @@
         <v>2.0</v>
       </c>
       <c r="F10" t="n">
-        <v>6.0779199827485915</v>
+        <v>5.089480062128999</v>
       </c>
       <c r="G10" t="n">
-        <v>11.308770572554618</v>
+        <v>0.5265579224240691</v>
       </c>
       <c r="H10" t="n">
-        <v>1.1011538739053233</v>
+        <v>1.251637177473392</v>
       </c>
       <c r="I10" t="n">
-        <v>4.835352438953284</v>
+        <v>5.094944682961728</v>
       </c>
       <c r="J10" t="n">
-        <v>2.8618683028897074</v>
+        <v>12.185505647084966</v>
       </c>
       <c r="K10" t="n">
-        <v>1.7075689082840269</v>
+        <v>0.34607585288479203</v>
       </c>
       <c r="L10" t="n">
-        <v>3.1581020604939747</v>
+        <v>27.66090308947151</v>
       </c>
     </row>
     <row r="11">
@@ -458,7 +458,7 @@
         <v>0.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1.1638570179731347</v>
+        <v>0.974581288492787</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -467,7 +467,7 @@
         <v>0.0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9259185521399905</v>
+        <v>0.9756277052479905</v>
       </c>
       <c r="J11" t="n">
         <v>0.0</v>
@@ -484,7 +484,7 @@
         <v>12.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C12" t="n">
         <v>1.5</v>
@@ -496,25 +496,25 @@
         <v>4.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1.939761696621891</v>
+        <v>1.6243021474879784</v>
       </c>
       <c r="G12" t="n">
-        <v>3.0156721526812316</v>
+        <v>0.14041544597975175</v>
       </c>
       <c r="H12" t="n">
-        <v>2.2023077478106465</v>
+        <v>2.503274354946784</v>
       </c>
       <c r="I12" t="n">
-        <v>1.543197586899984</v>
+        <v>1.6260461754133173</v>
       </c>
       <c r="J12" t="n">
-        <v>0.7631648807705886</v>
+        <v>3.249468172555991</v>
       </c>
       <c r="K12" t="n">
-        <v>3.4151378165680537</v>
+        <v>0.6921517057695841</v>
       </c>
       <c r="L12" t="n">
-        <v>0.8421605494650599</v>
+        <v>7.376240823859069</v>
       </c>
     </row>
     <row r="13">
@@ -522,7 +522,7 @@
         <v>13.0</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C13" t="n">
         <v>2.0</v>
@@ -534,25 +534,25 @@
         <v>6.0</v>
       </c>
       <c r="F13" t="n">
-        <v>2.586348928829188</v>
+        <v>2.165736196650638</v>
       </c>
       <c r="G13" t="n">
-        <v>3.0156721526812316</v>
+        <v>0.14041544597975175</v>
       </c>
       <c r="H13" t="n">
-        <v>3.30346162171597</v>
+        <v>3.7549115324201763</v>
       </c>
       <c r="I13" t="n">
-        <v>2.057596782533312</v>
+        <v>2.1680615672177566</v>
       </c>
       <c r="J13" t="n">
-        <v>0.7631648807705886</v>
+        <v>3.249468172555991</v>
       </c>
       <c r="K13" t="n">
-        <v>5.122706724852081</v>
+        <v>1.038227558654376</v>
       </c>
       <c r="L13" t="n">
-        <v>0.8421605494650599</v>
+        <v>7.376240823859069</v>
       </c>
     </row>
     <row r="14">
@@ -560,7 +560,7 @@
         <v>14.0</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C14" t="n">
         <v>1.2</v>
@@ -572,25 +572,25 @@
         <v>4.0</v>
       </c>
       <c r="F14" t="n">
-        <v>1.5518093572975127</v>
+        <v>1.2994417179903828</v>
       </c>
       <c r="G14" t="n">
-        <v>4.523508229021847</v>
+        <v>0.21062316896962763</v>
       </c>
       <c r="H14" t="n">
-        <v>2.2023077478106465</v>
+        <v>2.503274354946784</v>
       </c>
       <c r="I14" t="n">
-        <v>1.2345580695199871</v>
+        <v>1.300836940330654</v>
       </c>
       <c r="J14" t="n">
-        <v>1.144747321155883</v>
+        <v>4.874202258833987</v>
       </c>
       <c r="K14" t="n">
-        <v>3.4151378165680537</v>
+        <v>0.6921517057695841</v>
       </c>
       <c r="L14" t="n">
-        <v>1.2632408241975899</v>
+        <v>11.064361235788603</v>
       </c>
     </row>
     <row r="15">
@@ -610,25 +610,25 @@
         <v>6.0</v>
       </c>
       <c r="F15" t="n">
-        <v>1.5518093572975127</v>
+        <v>1.2994417179903828</v>
       </c>
       <c r="G15" t="n">
-        <v>7.539180381703079</v>
+        <v>0.3510386149493794</v>
       </c>
       <c r="H15" t="n">
-        <v>3.30346162171597</v>
+        <v>3.7549115324201763</v>
       </c>
       <c r="I15" t="n">
-        <v>1.2345580695199871</v>
+        <v>1.300836940330654</v>
       </c>
       <c r="J15" t="n">
-        <v>1.9079122019264716</v>
+        <v>8.123670431389979</v>
       </c>
       <c r="K15" t="n">
-        <v>5.122706724852081</v>
+        <v>1.038227558654376</v>
       </c>
       <c r="L15" t="n">
-        <v>2.10540137366265</v>
+        <v>18.440602059647674</v>
       </c>
     </row>
     <row r="16">
@@ -648,25 +648,25 @@
         <v>10.0</v>
       </c>
       <c r="F16" t="n">
-        <v>2.844983821712107</v>
+        <v>2.382309816315702</v>
       </c>
       <c r="G16" t="n">
-        <v>12.062688610724926</v>
+        <v>0.561661783919007</v>
       </c>
       <c r="H16" t="n">
-        <v>5.505769369526616</v>
+        <v>6.2581858873669605</v>
       </c>
       <c r="I16" t="n">
-        <v>2.2633564607866434</v>
+        <v>2.3848677239395326</v>
       </c>
       <c r="J16" t="n">
-        <v>3.0526595230823546</v>
+        <v>12.997872690223964</v>
       </c>
       <c r="K16" t="n">
-        <v>8.537844541420135</v>
+        <v>1.7303792644239602</v>
       </c>
       <c r="L16" t="n">
-        <v>3.3686421978602397</v>
+        <v>29.504963295436276</v>
       </c>
     </row>
     <row r="17">
@@ -686,25 +686,25 @@
         <v>8.0</v>
       </c>
       <c r="F17" t="n">
-        <v>9.828125929550913</v>
+        <v>8.229797547272424</v>
       </c>
       <c r="G17" t="n">
-        <v>9.047016458043695</v>
+        <v>0.42124633793925526</v>
       </c>
       <c r="H17" t="n">
-        <v>4.404615495621293</v>
+        <v>5.006548709893568</v>
       </c>
       <c r="I17" t="n">
-        <v>7.818867773626586</v>
+        <v>8.238633955427474</v>
       </c>
       <c r="J17" t="n">
-        <v>2.289494642311766</v>
+        <v>9.748404517667973</v>
       </c>
       <c r="K17" t="n">
-        <v>6.830275633136107</v>
+        <v>1.3843034115391681</v>
       </c>
       <c r="L17" t="n">
-        <v>2.5264816483951797</v>
+        <v>22.128722471577206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>